<commit_message>
se agregan pruebas de tipos de datos
</commit_message>
<xml_diff>
--- a/Importador.Excel.Tests/Resources/PruebaFechaCorrecta.xlsx
+++ b/Importador.Excel.Tests/Resources/PruebaFechaCorrecta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Orjuela\Documents\Temp\importador-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Orjuela\Documents\Temp\importador-excel\Importador.Excel.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{051BCE3D-9E36-4980-A0E4-EC94F0DD6A6A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B545F6-AF7A-4626-A161-7F19E04DF215}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{8AA5B533-058B-4AFB-9817-99C3129CBDE7}"/>
   </bookViews>
@@ -78,9 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,13 +396,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13436522-B273-47BE-B8B3-4F6547551C51}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -425,7 +429,11 @@
         <v>42923</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se Agregan las validaciones Faltantes
</commit_message>
<xml_diff>
--- a/Importador.Excel.Tests/Resources/PruebaFechaCorrecta.xlsx
+++ b/Importador.Excel.Tests/Resources/PruebaFechaCorrecta.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luis Orjuela\Documents\Temp\importador-excel\Importador.Excel.Tests\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fuentes\importador-excel\Importador.Excel.Tests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B545F6-AF7A-4626-A161-7F19E04DF215}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{8AA5B533-058B-4AFB-9817-99C3129CBDE7}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,8 +47,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +56,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -75,16 +86,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="EstiloLabel" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="SinEstilo" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,11 +411,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13436522-B273-47BE-B8B3-4F6547551C51}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,9 +445,6 @@
         <v>42923</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>